<commit_message>
Update data package at: 2023-09-20T14:28:50Z
</commit_message>
<xml_diff>
--- a/data-raw/FFP_acoes.xlsx
+++ b/data-raw/FFP_acoes.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26914"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\2.Programação e Normas\2023\PPAG 2023 e LOA 2023\Tabelas de Apoio - geração dos volumes 2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jackie\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{293BB599-3A1D-4D1F-A7BD-12603AC4E5D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{112FC2A9-1ED7-4505-8B8B-766373B99C00}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -17,26 +18,57 @@
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$C$58</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_SECOND_FORMAT" hidden="1">" "</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+  <si>
+    <t>COD_UO</t>
+  </si>
   <si>
     <t>ACAO</t>
   </si>
   <si>
+    <t>DESCRITIVO_ACAO</t>
+  </si>
+  <si>
+    <t>BENEFÍCIOS PREVIDENCIÁRIOS - SECOM</t>
+  </si>
+  <si>
+    <t>BENEFÍCIOS PREVIDENCIÁRIOS - CASA CIVIL</t>
+  </si>
+  <si>
     <t>BENEFÍCIOS PREVIDENCIÁRIOS - ARMBH</t>
   </si>
   <si>
     <t>BENEFÍCIOS PREVIDENCIÁRIOS - ESP-MG</t>
   </si>
   <si>
+    <t>BENEFÍCIOS PREVIDENCIÁRIOS - SEJUSP</t>
+  </si>
+  <si>
     <t>BENEFÍCIOS PREVIDENCIÁRIOS - ARSAE-MG</t>
   </si>
   <si>
@@ -55,6 +87,9 @@
     <t>BENEFÍCIOS PREVIDENCIÁRIOS - TJMG</t>
   </si>
   <si>
+    <t>BENEFÍCIOS PREVIDENCIÁRIOS - MPMG</t>
+  </si>
+  <si>
     <t>BENEFÍCIOS PREVIDENCIÁRIOS - TJMMG</t>
   </si>
   <si>
@@ -70,6 +105,9 @@
     <t>BENEFÍCIOS PREVIDENCIÁRIOS - ARMVA</t>
   </si>
   <si>
+    <t>BENEFÍCIOS PREVIDENCIÁRIOS - SEC GERAL</t>
+  </si>
+  <si>
     <t>BENEFÍCIOS PREVIDENCIÁRIOS - CGE</t>
   </si>
   <si>
@@ -94,12 +132,21 @@
     <t>BENEFÍCIOS PREVIDENCIÁRIOS - OGE</t>
   </si>
   <si>
+    <t>BENEFÍCIOS PREVIDENCIÁRIOS - SEDE</t>
+  </si>
+  <si>
     <t>BENEFÍCIOS PREVIDENCIÁRIOS - SEAPA</t>
   </si>
   <si>
+    <t>BENEFÍCIOS PREVIDENCIÁRIOS - SECULT</t>
+  </si>
+  <si>
     <t>BENEFÍCIOS PREVIDENCIÁRIOS - UEMG</t>
   </si>
   <si>
+    <t>BENEFÍCIOS PREVIDENCIÁRIOS - SEINFRA</t>
+  </si>
+  <si>
     <t>BENEFÍCIOS PREVIDENCIÁRIOS - SEMAD</t>
   </si>
   <si>
@@ -130,6 +177,9 @@
     <t>BENEFÍCIOS PREVIDENCIÁRIOS - TV MINAS</t>
   </si>
   <si>
+    <t>BENEFÍCIOS PREVIDENCIÁRIOS - DEER</t>
+  </si>
+  <si>
     <t>BENEFÍCIOS PREVIDENCIÁRIOS - FUNED</t>
   </si>
   <si>
@@ -173,40 +223,13 @@
   </si>
   <si>
     <t>BENEFÍCIOS PREVIDENCIÁRIOS - SES</t>
-  </si>
-  <si>
-    <t>COD_UO</t>
-  </si>
-  <si>
-    <t>DESCRITIVO_ACAO</t>
-  </si>
-  <si>
-    <t>BENEFÍCIOS PREVIDENCIÁRIOS - DEER</t>
-  </si>
-  <si>
-    <t>BENEFÍCIOS PREVIDENCIÁRIOS - SEC GERAL</t>
-  </si>
-  <si>
-    <t>BENEFÍCIOS PREVIDENCIÁRIOS - SEJUSP</t>
-  </si>
-  <si>
-    <t>BENEFÍCIOS PREVIDENCIÁRIOS - SEDE</t>
-  </si>
-  <si>
-    <t>BENEFÍCIOS PREVIDENCIÁRIOS - SECULT</t>
-  </si>
-  <si>
-    <t>BENEFÍCIOS PREVIDENCIÁRIOS - SEINFRA</t>
-  </si>
-  <si>
-    <t>BENEFÍCIOS PREVIDENCIÁRIOS - MPMG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -684,9 +707,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -718,10 +740,10 @@
     <cellStyle name="Ênfase5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Ênfase6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Incorreto" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Neutra" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Neutro" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Nota" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Ruim" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Saída" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Texto de Aviso" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Texto Explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
@@ -757,7 +779,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -774,9 +796,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -814,9 +836,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -851,7 +873,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -886,7 +908,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1059,669 +1081,719 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C56"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="46.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="46.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1711</v>
+      </c>
+      <c r="B2">
+        <v>7005</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>1721</v>
+      </c>
+      <c r="B3">
+        <v>7009</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>2431</v>
+      </c>
+      <c r="B4">
+        <v>7011</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>1541</v>
+      </c>
+      <c r="B5">
+        <v>7012</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>1451</v>
+      </c>
+      <c r="B6">
+        <v>7014</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>2441</v>
+      </c>
+      <c r="B7">
+        <v>7015</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>1071</v>
+      </c>
+      <c r="B8">
+        <v>7017</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>1081</v>
+      </c>
+      <c r="B9">
+        <v>7018</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>2071</v>
+      </c>
+      <c r="B10">
+        <v>7022</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>1011</v>
+      </c>
+      <c r="B11">
+        <v>7027</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>1031</v>
+      </c>
+      <c r="B12">
+        <v>7028</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>1091</v>
+      </c>
+      <c r="B13">
+        <v>7031</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>1051</v>
+      </c>
+      <c r="B14">
+        <v>7032</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>1021</v>
+      </c>
+      <c r="B15">
+        <v>7033</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>1441</v>
+      </c>
+      <c r="B16">
+        <v>7034</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>1191</v>
+      </c>
+      <c r="B17">
+        <v>7037</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>2461</v>
+      </c>
+      <c r="B18">
+        <v>7039</v>
+      </c>
+      <c r="C18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>1631</v>
+      </c>
+      <c r="B19">
+        <v>7040</v>
+      </c>
+      <c r="C19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>1521</v>
+      </c>
+      <c r="B20">
+        <v>7044</v>
+      </c>
+      <c r="C20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>2311</v>
+      </c>
+      <c r="B21">
+        <v>7046</v>
+      </c>
+      <c r="C21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22">
+        <v>2331</v>
+      </c>
+      <c r="B22">
+        <v>7047</v>
+      </c>
+      <c r="C22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>1511</v>
+      </c>
+      <c r="B23">
+        <v>7048</v>
+      </c>
+      <c r="C23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>1501</v>
+      </c>
+      <c r="B24">
+        <v>7049</v>
+      </c>
+      <c r="C24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25">
+        <v>1491</v>
+      </c>
+      <c r="B25">
+        <v>7051</v>
+      </c>
+      <c r="C25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26">
+        <v>1481</v>
+      </c>
+      <c r="B26">
+        <v>7052</v>
+      </c>
+      <c r="C26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27">
+        <v>1101</v>
+      </c>
+      <c r="B27">
+        <v>7055</v>
+      </c>
+      <c r="C27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28">
+        <v>1221</v>
+      </c>
+      <c r="B28">
+        <v>7056</v>
+      </c>
+      <c r="C28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29">
+        <v>1231</v>
+      </c>
+      <c r="B29">
+        <v>7058</v>
+      </c>
+      <c r="C29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30">
+        <v>1271</v>
+      </c>
+      <c r="B30">
+        <v>7059</v>
+      </c>
+      <c r="C30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31">
+        <v>2351</v>
+      </c>
+      <c r="B31">
+        <v>7060</v>
+      </c>
+      <c r="C31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32">
+        <v>1301</v>
+      </c>
+      <c r="B32">
+        <v>7061</v>
+      </c>
+      <c r="C32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33">
+        <v>1371</v>
+      </c>
+      <c r="B33">
+        <v>7063</v>
+      </c>
+      <c r="C33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34">
+        <v>1251</v>
+      </c>
+      <c r="B34">
+        <v>7064</v>
+      </c>
+      <c r="C34" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35">
+        <v>1401</v>
+      </c>
+      <c r="B35">
+        <v>7065</v>
+      </c>
+      <c r="C35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36">
+        <v>2371</v>
+      </c>
+      <c r="B36">
+        <v>7088</v>
+      </c>
+      <c r="C36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37">
+        <v>2151</v>
+      </c>
+      <c r="B37">
+        <v>7089</v>
+      </c>
+      <c r="C37" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38">
+        <v>2161</v>
+      </c>
+      <c r="B38">
+        <v>7091</v>
+      </c>
+      <c r="C38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39">
+        <v>2171</v>
+      </c>
+      <c r="B39">
+        <v>7094</v>
+      </c>
+      <c r="C39" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40">
+        <v>2181</v>
+      </c>
+      <c r="B40">
+        <v>7096</v>
+      </c>
+      <c r="C40" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41">
+        <v>2201</v>
+      </c>
+      <c r="B41">
+        <v>7104</v>
+      </c>
+      <c r="C41" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42">
+        <v>2211</v>
+      </c>
+      <c r="B42">
+        <v>7105</v>
+      </c>
+      <c r="C42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43">
+        <v>2301</v>
+      </c>
+      <c r="B43">
+        <v>7205</v>
+      </c>
+      <c r="C43" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44">
+        <v>2261</v>
+      </c>
+      <c r="B44">
+        <v>7209</v>
+      </c>
+      <c r="C44" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45">
+        <v>2271</v>
+      </c>
+      <c r="B45">
+        <v>7225</v>
+      </c>
+      <c r="C45" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46">
+        <v>2321</v>
+      </c>
+      <c r="B46">
+        <v>7312</v>
+      </c>
+      <c r="C46" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47">
+        <v>2091</v>
+      </c>
+      <c r="B47">
+        <v>7428</v>
+      </c>
+      <c r="C47" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48">
+        <v>2101</v>
+      </c>
+      <c r="B48">
+        <v>7473</v>
+      </c>
+      <c r="C48" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49">
+        <v>2241</v>
+      </c>
+      <c r="B49">
+        <v>7484</v>
+      </c>
+      <c r="C49" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1451</v>
-      </c>
-      <c r="B2" s="1">
-        <v>7014</v>
-      </c>
-      <c r="C2" s="1" t="s">
+    <row r="50" spans="1:3">
+      <c r="A50">
+        <v>2251</v>
+      </c>
+      <c r="B50">
+        <v>7529</v>
+      </c>
+      <c r="C50" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51">
+        <v>2281</v>
+      </c>
+      <c r="B51">
+        <v>7586</v>
+      </c>
+      <c r="C51" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52">
+        <v>2041</v>
+      </c>
+      <c r="B52">
+        <v>7617</v>
+      </c>
+      <c r="C52" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2431</v>
-      </c>
-      <c r="B3" s="1">
-        <v>7011</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>1541</v>
-      </c>
-      <c r="B4" s="1">
-        <v>7012</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>2441</v>
-      </c>
-      <c r="B5" s="1">
-        <v>7015</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>1071</v>
-      </c>
-      <c r="B6" s="1">
-        <v>7017</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>1081</v>
-      </c>
-      <c r="B7" s="1">
-        <v>7018</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>2071</v>
-      </c>
-      <c r="B8" s="1">
-        <v>7022</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>1011</v>
-      </c>
-      <c r="B9" s="1">
-        <v>7027</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>1031</v>
-      </c>
-      <c r="B10" s="1">
-        <v>7028</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>1091</v>
-      </c>
-      <c r="B11" s="1">
-        <v>7031</v>
-      </c>
-      <c r="C11" s="1" t="s">
+    <row r="53" spans="1:3">
+      <c r="A53">
+        <v>2061</v>
+      </c>
+      <c r="B53">
+        <v>7722</v>
+      </c>
+      <c r="C53" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54">
+        <v>2011</v>
+      </c>
+      <c r="B54">
+        <v>7725</v>
+      </c>
+      <c r="C54" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55">
+        <v>2121</v>
+      </c>
+      <c r="B55">
+        <v>7840</v>
+      </c>
+      <c r="C55" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56">
+        <v>2421</v>
+      </c>
+      <c r="B56">
+        <v>7939</v>
+      </c>
+      <c r="C56" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>1051</v>
-      </c>
-      <c r="B12" s="1">
-        <v>7032</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>1021</v>
-      </c>
-      <c r="B13" s="1">
-        <v>7033</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>1441</v>
-      </c>
-      <c r="B14" s="1">
-        <v>7034</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>1191</v>
-      </c>
-      <c r="B15" s="1">
-        <v>7037</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>2461</v>
-      </c>
-      <c r="B16" s="1">
-        <v>7039</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>1631</v>
-      </c>
-      <c r="B17" s="1">
-        <v>7040</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>1521</v>
-      </c>
-      <c r="B18" s="1">
-        <v>7044</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>2311</v>
-      </c>
-      <c r="B19" s="1">
-        <v>7046</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>2331</v>
-      </c>
-      <c r="B20" s="1">
-        <v>7047</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>1511</v>
-      </c>
-      <c r="B21" s="1">
-        <v>7048</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>1501</v>
-      </c>
-      <c r="B22" s="1">
-        <v>7049</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>1491</v>
-      </c>
-      <c r="B23" s="1">
-        <v>7051</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>1481</v>
-      </c>
-      <c r="B24" s="1">
-        <v>7052</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>1101</v>
-      </c>
-      <c r="B25" s="1">
-        <v>7055</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>1221</v>
-      </c>
-      <c r="B26" s="1">
-        <v>7056</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>1231</v>
-      </c>
-      <c r="B27" s="1">
-        <v>7058</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>1271</v>
-      </c>
-      <c r="B28" s="1">
-        <v>7059</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>2351</v>
-      </c>
-      <c r="B29" s="1">
-        <v>7060</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>1301</v>
-      </c>
-      <c r="B30" s="1">
-        <v>7061</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>1371</v>
-      </c>
-      <c r="B31" s="1">
-        <v>7063</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>1251</v>
-      </c>
-      <c r="B32" s="1">
-        <v>7064</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>1401</v>
-      </c>
-      <c r="B33" s="1">
-        <v>7065</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>2371</v>
-      </c>
-      <c r="B34" s="1">
-        <v>7088</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>2151</v>
-      </c>
-      <c r="B35" s="1">
-        <v>7089</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>2161</v>
-      </c>
-      <c r="B36" s="1">
-        <v>7091</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <v>2171</v>
-      </c>
-      <c r="B37" s="1">
-        <v>7094</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
-        <v>2181</v>
-      </c>
-      <c r="B38" s="1">
-        <v>7096</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>2201</v>
-      </c>
-      <c r="B39" s="1">
-        <v>7104</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <v>2211</v>
-      </c>
-      <c r="B40" s="1">
-        <v>7105</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>2301</v>
-      </c>
-      <c r="B41" s="1">
-        <v>7205</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
-        <v>2261</v>
-      </c>
-      <c r="B42" s="1">
-        <v>7209</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
-        <v>2271</v>
-      </c>
-      <c r="B43" s="1">
-        <v>7225</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
-        <v>2321</v>
-      </c>
-      <c r="B44" s="1">
-        <v>7312</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
-        <v>2091</v>
-      </c>
-      <c r="B45" s="1">
-        <v>7428</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
-        <v>2101</v>
-      </c>
-      <c r="B46" s="1">
-        <v>7473</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
-        <v>2241</v>
-      </c>
-      <c r="B47" s="1">
-        <v>7484</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
-        <v>2251</v>
-      </c>
-      <c r="B48" s="1">
-        <v>7529</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
-        <v>2281</v>
-      </c>
-      <c r="B49" s="1">
-        <v>7586</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
-        <v>2041</v>
-      </c>
-      <c r="B50" s="1">
-        <v>7617</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
-        <v>2061</v>
-      </c>
-      <c r="B51" s="1">
-        <v>7722</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
-        <v>2011</v>
-      </c>
-      <c r="B52" s="1">
-        <v>7725</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
-        <v>2121</v>
-      </c>
-      <c r="B53" s="1">
-        <v>7840</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
-        <v>2421</v>
-      </c>
-      <c r="B54" s="1">
-        <v>7939</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
+    <row r="57" spans="1:3">
+      <c r="A57">
         <v>1261</v>
       </c>
-      <c r="B55" s="1">
+      <c r="B57">
         <v>7957</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
+      <c r="C57" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58">
         <v>4291</v>
       </c>
-      <c r="B56" s="1">
+      <c r="B58">
         <v>7959</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>48</v>
+      <c r="C58" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:C58">
+    <sortCondition ref="B1:B58"/>
+  </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B08D58FADB61F04EBBB4F355C06EFBED" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4e1f47f591d2cee6122bef25da059db4">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6f4338ef-addb-4c87-aefe-1895241b335f" xmlns:ns3="b91e7f20-fe0a-487d-91a9-605ac1c64acf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="856a76bd91320367711680b85ef754cf" ns2:_="" ns3:_="">
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b91e7f20-fe0a-487d-91a9-605ac1c64acf" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6f4338ef-addb-4c87-aefe-1895241b335f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="b91e7f20-fe0a-487d-91a9-605ac1c64acf">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <MediaLengthInSeconds xmlns="6f4338ef-addb-4c87-aefe-1895241b335f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B08D58FADB61F04EBBB4F355C06EFBED" ma:contentTypeVersion="17" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="c170a06b81d8b923cbfe6a63de8ee1c9">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6f4338ef-addb-4c87-aefe-1895241b335f" xmlns:ns3="b91e7f20-fe0a-487d-91a9-605ac1c64acf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="844dfdedaab7989660d9d802f918fcda" ns2:_="" ns3:_="">
     <xsd:import namespace="6f4338ef-addb-4c87-aefe-1895241b335f"/>
     <xsd:import namespace="b91e7f20-fe0a-487d-91a9-605ac1c64acf"/>
     <xsd:element name="properties">
@@ -1800,7 +1872,7 @@
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="19" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="917d32f3-4fa4-4f5b-a8d0-62dbd3d265b9" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="19" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Marcações de imagem" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="917d32f3-4fa4-4f5b-a8d0-62dbd3d265b9" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -1831,7 +1903,7 @@
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="b91e7f20-fe0a-487d-91a9-605ac1c64acf" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="10" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="10" nillable="true" ma:displayName="Compartilhado com" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -1850,7 +1922,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="11" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="11" nillable="true" ma:displayName="Detalhes de Compartilhado Com" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -1878,8 +1950,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de Conteúdo"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -1968,34 +2040,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b91e7f20-fe0a-487d-91a9-605ac1c64acf" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6f4338ef-addb-4c87-aefe-1895241b335f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{510EBCBE-0446-4C1F-A0FD-8AB4006BE7F4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1DB9620-CC88-4257-8480-C321EF6EFF37}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C84EB41-A097-4B53-9DB5-E53D03DA3C26}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7C923F2-A4FA-4B59-9477-1E7A98C0125A}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3687408F-E4F6-42D4-B829-435F7DFC4503}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87E3933F-A2E5-4DC6-92D7-456B067CD7DF}"/>
 </file>
</xml_diff>

<commit_message>
Update data package at: 2024-09-24T14:20:57Z
</commit_message>
<xml_diff>
--- a/data-raw/FFP_acoes.xlsx
+++ b/data-raw/FFP_acoes.xlsx
@@ -1786,14 +1786,13 @@
         <AccountType/>
       </UserInfo>
     </SharedWithUsers>
-    <MediaLengthInSeconds xmlns="6f4338ef-addb-4c87-aefe-1895241b335f" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B08D58FADB61F04EBBB4F355C06EFBED" ma:contentTypeVersion="17" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="c170a06b81d8b923cbfe6a63de8ee1c9">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6f4338ef-addb-4c87-aefe-1895241b335f" xmlns:ns3="b91e7f20-fe0a-487d-91a9-605ac1c64acf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="844dfdedaab7989660d9d802f918fcda" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B08D58FADB61F04EBBB4F355C06EFBED" ma:contentTypeVersion="18" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="1b889f39a240c2e855286b20cf95d05e">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6f4338ef-addb-4c87-aefe-1895241b335f" xmlns:ns3="b91e7f20-fe0a-487d-91a9-605ac1c64acf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="902f44b668f40cdc6ccc2fe791adf365" ns2:_="" ns3:_="">
     <xsd:import namespace="6f4338ef-addb-4c87-aefe-1895241b335f"/>
     <xsd:import namespace="b91e7f20-fe0a-487d-91a9-605ac1c64acf"/>
     <xsd:element name="properties">
@@ -1818,6 +1817,7 @@
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -1897,6 +1897,11 @@
     <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="24" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="25" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -2049,5 +2054,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87E3933F-A2E5-4DC6-92D7-456B067CD7DF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B73CBC72-94FB-4749-B4A7-5630AEE7F21E}"/>
 </file>
</xml_diff>

<commit_message>
Update data package at: 2025-09-26T17:21:54Z
</commit_message>
<xml_diff>
--- a/data-raw/FFP_acoes.xlsx
+++ b/data-raw/FFP_acoes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29301"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jackie\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{293BB599-3A1D-4D1F-A7BD-12603AC4E5D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{112FC2A9-1ED7-4505-8B8B-766373B99C00}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{293BB599-3A1D-4D1F-A7BD-12603AC4E5D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61D68A63-ED1E-4C14-9962-56DAA0DC9353}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>COD_UO</t>
   </si>
@@ -223,13 +223,16 @@
   </si>
   <si>
     <t>BENEFÍCIOS PREVIDENCIÁRIOS - SES</t>
+  </si>
+  <si>
+    <t>BENEFÍCIOS PREVIDENCIÁRIOS - ARTEMIG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -365,8 +368,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -544,6 +553,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -707,8 +722,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1082,9 +1098,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59:C59"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1728,6 +1746,17 @@
       </c>
       <c r="C58" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="1">
+        <v>2011</v>
+      </c>
+      <c r="B59" s="1">
+        <v>7020</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1764,35 +1793,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b91e7f20-fe0a-487d-91a9-605ac1c64acf" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6f4338ef-addb-4c87-aefe-1895241b335f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="b91e7f20-fe0a-487d-91a9-605ac1c64acf">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B08D58FADB61F04EBBB4F355C06EFBED" ma:contentTypeVersion="18" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="1b889f39a240c2e855286b20cf95d05e">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6f4338ef-addb-4c87-aefe-1895241b335f" xmlns:ns3="b91e7f20-fe0a-487d-91a9-605ac1c64acf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="902f44b668f40cdc6ccc2fe791adf365" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B08D58FADB61F04EBBB4F355C06EFBED" ma:contentTypeVersion="19" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="7797dc5feb179b4da55a9ebddd321181">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6f4338ef-addb-4c87-aefe-1895241b335f" xmlns:ns3="b91e7f20-fe0a-487d-91a9-605ac1c64acf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="90078f443198b6d5c0fd169535a443b9" ns2:_="" ns3:_="">
     <xsd:import namespace="6f4338ef-addb-4c87-aefe-1895241b335f"/>
     <xsd:import namespace="b91e7f20-fe0a-487d-91a9-605ac1c64acf"/>
     <xsd:element name="properties">
@@ -1818,6 +1820,7 @@
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceBillingMetadata" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -1900,6 +1903,11 @@
       </xsd:simpleType>
     </xsd:element>
     <xsd:element name="MediaServiceSearchProperties" ma:index="25" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceBillingMetadata" ma:index="26" nillable="true" ma:displayName="MediaServiceBillingMetadata" ma:hidden="true" ma:internalName="MediaServiceBillingMetadata" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
@@ -2045,14 +2053,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b91e7f20-fe0a-487d-91a9-605ac1c64acf" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6f4338ef-addb-4c87-aefe-1895241b335f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="b91e7f20-fe0a-487d-91a9-605ac1c64acf">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBB7F238-CDE3-461E-8F60-E82D00978859}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1DB9620-CC88-4257-8480-C321EF6EFF37}"/>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7C923F2-A4FA-4B59-9477-1E7A98C0125A}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B73CBC72-94FB-4749-B4A7-5630AEE7F21E}"/>
 </file>
</xml_diff>

<commit_message>
Update data package at: 2025-09-29T17:26:08Z
</commit_message>
<xml_diff>
--- a/data-raw/FFP_acoes.xlsx
+++ b/data-raw/FFP_acoes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29301"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jackie\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cecad365.sharepoint.com/sites/Splor/Documentos Compartilhados/General/@dcppn/DCPPN 2026/PPAG e LOA 2026/material de apoio/material de apoio - gerar volumes/2026/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{293BB599-3A1D-4D1F-A7BD-12603AC4E5D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61D68A63-ED1E-4C14-9962-56DAA0DC9353}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{293BB599-3A1D-4D1F-A7BD-12603AC4E5D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C49F7F53-BA0F-4271-AA20-D647FF57380A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$C$58</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$C$59</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_SECOND_FORMAT" hidden="1">" "</definedName>
   </definedNames>
@@ -232,7 +232,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="19">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -809,6 +809,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/namedSheetViews/namedSheetView1.xml><?xml version="1.0" encoding="utf-8"?>
+<namedSheetViews xmlns="http://schemas.microsoft.com/office/spreadsheetml/2019/namedsheetviews" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1098,19 +1102,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:C59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59:C59"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" customWidth="1"/>
     <col min="3" max="3" width="46.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1121,7 +1126,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1711</v>
       </c>
@@ -1132,7 +1137,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1721</v>
       </c>
@@ -1143,7 +1148,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2431</v>
       </c>
@@ -1154,7 +1159,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1541</v>
       </c>
@@ -1165,7 +1170,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1451</v>
       </c>
@@ -1176,7 +1181,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2441</v>
       </c>
@@ -1187,7 +1192,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1071</v>
       </c>
@@ -1198,7 +1203,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1081</v>
       </c>
@@ -1209,7 +1214,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2071</v>
       </c>
@@ -1220,7 +1225,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1011</v>
       </c>
@@ -1231,7 +1236,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1031</v>
       </c>
@@ -1242,7 +1247,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1091</v>
       </c>
@@ -1253,7 +1258,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1051</v>
       </c>
@@ -1264,7 +1269,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1021</v>
       </c>
@@ -1275,7 +1280,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1441</v>
       </c>
@@ -1286,7 +1291,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1191</v>
       </c>
@@ -1297,7 +1302,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2461</v>
       </c>
@@ -1308,7 +1313,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1631</v>
       </c>
@@ -1319,7 +1324,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1521</v>
       </c>
@@ -1330,7 +1335,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2311</v>
       </c>
@@ -1341,7 +1346,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2331</v>
       </c>
@@ -1352,7 +1357,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1511</v>
       </c>
@@ -1363,7 +1368,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1501</v>
       </c>
@@ -1374,7 +1379,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1491</v>
       </c>
@@ -1385,7 +1390,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1481</v>
       </c>
@@ -1396,7 +1401,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1101</v>
       </c>
@@ -1407,7 +1412,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1221</v>
       </c>
@@ -1418,7 +1423,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1231</v>
       </c>
@@ -1429,7 +1434,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1271</v>
       </c>
@@ -1440,7 +1445,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2351</v>
       </c>
@@ -1451,7 +1456,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1301</v>
       </c>
@@ -1462,7 +1467,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1371</v>
       </c>
@@ -1473,7 +1478,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1251</v>
       </c>
@@ -1484,7 +1489,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1401</v>
       </c>
@@ -1495,7 +1500,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2371</v>
       </c>
@@ -1506,7 +1511,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2151</v>
       </c>
@@ -1517,7 +1522,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2161</v>
       </c>
@@ -1528,7 +1533,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2171</v>
       </c>
@@ -1539,7 +1544,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2181</v>
       </c>
@@ -1550,7 +1555,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2201</v>
       </c>
@@ -1561,7 +1566,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2211</v>
       </c>
@@ -1572,7 +1577,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2301</v>
       </c>
@@ -1583,7 +1588,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2261</v>
       </c>
@@ -1594,7 +1599,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2271</v>
       </c>
@@ -1605,7 +1610,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2321</v>
       </c>
@@ -1616,7 +1621,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2091</v>
       </c>
@@ -1627,7 +1632,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2101</v>
       </c>
@@ -1638,7 +1643,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2241</v>
       </c>
@@ -1649,7 +1654,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2251</v>
       </c>
@@ -1660,7 +1665,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2281</v>
       </c>
@@ -1671,7 +1676,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2041</v>
       </c>
@@ -1682,7 +1687,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2061</v>
       </c>
@@ -1693,7 +1698,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2011</v>
       </c>
@@ -1704,7 +1709,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2121</v>
       </c>
@@ -1715,7 +1720,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2421</v>
       </c>
@@ -1726,7 +1731,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>1261</v>
       </c>
@@ -1737,7 +1742,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>4291</v>
       </c>
@@ -1748,9 +1753,9 @@
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>2011</v>
+        <v>2471</v>
       </c>
       <c r="B59" s="1">
         <v>7020</v>
@@ -1760,6 +1765,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C59" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="BENEFÍCIOS PREVIDENCIÁRIOS - ARTEMIG"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:C58">
     <sortCondition ref="B1:B58"/>
   </sortState>
@@ -1774,7 +1786,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -1786,13 +1798,40 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b91e7f20-fe0a-487d-91a9-605ac1c64acf" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6f4338ef-addb-4c87-aefe-1895241b335f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="b91e7f20-fe0a-487d-91a9-605ac1c64acf">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B08D58FADB61F04EBBB4F355C06EFBED" ma:contentTypeVersion="19" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="7797dc5feb179b4da55a9ebddd321181">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6f4338ef-addb-4c87-aefe-1895241b335f" xmlns:ns3="b91e7f20-fe0a-487d-91a9-605ac1c64acf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="90078f443198b6d5c0fd169535a443b9" ns2:_="" ns3:_="">
     <xsd:import namespace="6f4338ef-addb-4c87-aefe-1895241b335f"/>
@@ -2053,41 +2092,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b91e7f20-fe0a-487d-91a9-605ac1c64acf" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6f4338ef-addb-4c87-aefe-1895241b335f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="b91e7f20-fe0a-487d-91a9-605ac1c64acf">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBB7F238-CDE3-461E-8F60-E82D00978859}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7C923F2-A4FA-4B59-9477-1E7A98C0125A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b91e7f20-fe0a-487d-91a9-605ac1c64acf"/>
+    <ds:schemaRef ds:uri="6f4338ef-addb-4c87-aefe-1895241b335f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1DB9620-CC88-4257-8480-C321EF6EFF37}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1DB9620-CC88-4257-8480-C321EF6EFF37}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7C923F2-A4FA-4B59-9477-1E7A98C0125A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBB7F238-CDE3-461E-8F60-E82D00978859}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6f4338ef-addb-4c87-aefe-1895241b335f"/>
+    <ds:schemaRef ds:uri="b91e7f20-fe0a-487d-91a9-605ac1c64acf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>